<commit_message>
feat: Add report prototype
</commit_message>
<xml_diff>
--- a/3주차/result.xlsx
+++ b/3주차/result.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\lkh116\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - 서울대학교\수업\18학년도2학기\네트워크프로토콜및설계\과제\3주차\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{03AF1B81-3118-416C-AF24-C1173ABD32C8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0B2DC8BB-16A9-41CB-9F6A-524A21861FE5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12180" xr2:uid="{7F0D66D6-49DA-480B-8CDE-28007FCE08EF}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>rate</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -43,11 +43,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>On_send</t>
+    <t>Radio_on</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>On_recv</t>
+    <t>total</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -150,7 +150,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" altLang="ko-KR"/>
-              <a:t>Sender</a:t>
+              <a:t>Tx node</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -230,10 +230,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>Sheet1!$A$2:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -253,6 +253,9 @@
                   <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>256</c:v>
                 </c:pt>
               </c:numCache>
@@ -260,10 +263,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$8</c:f>
+              <c:f>Sheet1!$B$2:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>4.93</c:v>
                 </c:pt>
@@ -283,6 +286,9 @@
                   <c:v>0.19</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0.08</c:v>
                 </c:pt>
               </c:numCache>
@@ -304,7 +310,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>On_send</c:v>
+                  <c:v>Radio_on</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -335,10 +341,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>Sheet1!$A$2:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -358,6 +364,9 @@
                   <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>256</c:v>
                 </c:pt>
               </c:numCache>
@@ -365,10 +374,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$8</c:f>
+              <c:f>Sheet1!$D$2:$D$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>9.44</c:v>
                 </c:pt>
@@ -388,6 +397,9 @@
                   <c:v>6.01</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>11.47</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>22.61</c:v>
                 </c:pt>
               </c:numCache>
@@ -653,8 +665,13 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" altLang="ko-KR"/>
-              <a:t>Receiver</a:t>
+              <a:t>Rx</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" baseline="0"/>
+              <a:t> node</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" altLang="ko-KR"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -756,6 +773,9 @@
                   <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>256</c:v>
                 </c:pt>
               </c:numCache>
@@ -786,6 +806,9 @@
                   <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0.04</c:v>
                 </c:pt>
               </c:numCache>
@@ -807,7 +830,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>On_recv</c:v>
+                  <c:v>Radio_on</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -861,6 +884,9 @@
                   <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>256</c:v>
                 </c:pt>
               </c:numCache>
@@ -891,6 +917,9 @@
                   <c:v>5.7</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>11.26</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>22.71</c:v>
                 </c:pt>
               </c:numCache>
@@ -1121,6 +1150,354 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ko-KR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ko-KR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$2:$H$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>9.69</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.4799999999999995</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.88</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.1500000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.71</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22.73</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45.32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-61CD-4471-BCFD-34CDDF587D78}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="518351704"/>
+        <c:axId val="518356296"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="518351704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="518356296"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="518356296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="518351704"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ko-KR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1201,6 +1578,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1718,6 +2135,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2302,6 +3235,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="차트 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{06C353BA-D68E-451B-B8D4-F19B179D825A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2607,15 +3576,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CB23078-3817-4F9C-9CFE-6DA1708DD4BF}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+      <selection activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2629,13 +3598,16 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
       </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2</v>
       </c>
@@ -2654,8 +3626,12 @@
       <c r="F2">
         <v>4.84</v>
       </c>
+      <c r="H2">
+        <f>D2+E2</f>
+        <v>9.69</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>4</v>
       </c>
@@ -2674,8 +3650,12 @@
       <c r="F3">
         <v>2.74</v>
       </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H9" si="0">D3+E3</f>
+        <v>5.4799999999999995</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>8</v>
       </c>
@@ -2694,8 +3674,12 @@
       <c r="F4">
         <v>1.94</v>
       </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>3.88</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>16</v>
       </c>
@@ -2714,8 +3698,12 @@
       <c r="F5">
         <v>2.08</v>
       </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>4.1500000000000004</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>32</v>
       </c>
@@ -2734,8 +3722,12 @@
       <c r="F6">
         <v>3.2</v>
       </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>6.4</v>
+      </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>64</v>
       </c>
@@ -2754,30 +3746,63 @@
       <c r="F7">
         <v>5.85</v>
       </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>11.71</v>
+      </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
+        <v>128</v>
+      </c>
+      <c r="B8">
+        <v>0.11</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>11.47</v>
+      </c>
+      <c r="E8">
+        <v>11.26</v>
+      </c>
+      <c r="F8">
+        <v>11.38</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>22.73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9">
         <v>256</v>
       </c>
-      <c r="B8">
+      <c r="B9">
         <v>0.08</v>
       </c>
-      <c r="C8">
+      <c r="C9">
         <v>0.04</v>
       </c>
-      <c r="D8">
+      <c r="D9">
         <v>22.61</v>
       </c>
-      <c r="E8">
+      <c r="E9">
         <v>22.71</v>
       </c>
-      <c r="F8">
+      <c r="F9">
         <v>22.66</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>45.32</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>